<commit_message>
Changed ProtectedSite wordnet mapping
</commit_message>
<xml_diff>
--- a/wordnet_lexycal_mapping.xlsx
+++ b/wordnet_lexycal_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Magistrale\KDI\REPO\kdi_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8249E98C-E43D-4E24-9AAF-EF960DA82E9D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37821B87-FA52-44EE-99A4-522844FF51BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datatype_properties" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="176">
   <si>
     <t>domain_word</t>
   </si>
@@ -392,9 +392,6 @@
     <t>ProtectedSite</t>
   </si>
   <si>
-    <t>a particular environment or walk of life</t>
-  </si>
-  <si>
     <t>TransportationPoint</t>
   </si>
   <si>
@@ -524,9 +521,6 @@
     <t>country, state, land</t>
   </si>
   <si>
-    <t>sphere, domain, area, orbit, field, arena</t>
-  </si>
-  <si>
     <t>transportation system, transportation, transit</t>
   </si>
   <si>
@@ -552,6 +546,15 @@
   </si>
   <si>
     <t>contact</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>park, parkland</t>
+  </si>
+  <si>
+    <t>a large area of land preserved in its natural state as public property</t>
   </si>
 </sst>
 </file>
@@ -598,8 +601,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -985,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1421,19 +1425,19 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C24">
         <v>6271913</v>
       </c>
       <c r="D24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -1743,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1821,7 +1825,7 @@
         <v>8562388</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" t="s">
         <v>115</v>
@@ -1855,16 +1859,16 @@
         <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6">
-        <v>14537641</v>
-      </c>
-      <c r="D6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" t="s">
-        <v>121</v>
+        <v>173</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8632724</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -1872,19 +1876,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
         <v>122</v>
-      </c>
-      <c r="B7" t="s">
-        <v>123</v>
       </c>
       <c r="C7">
         <v>4480667</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -1892,19 +1896,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8">
         <v>2695091</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -1912,19 +1916,19 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9">
         <v>2695091</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -1932,16 +1936,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" t="s">
         <v>128</v>
-      </c>
-      <c r="B10" t="s">
-        <v>129</v>
       </c>
       <c r="C10">
         <v>8534954</v>
       </c>
       <c r="E10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -1949,19 +1953,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
         <v>131</v>
-      </c>
-      <c r="B11" t="s">
-        <v>132</v>
       </c>
       <c r="C11">
         <v>8656633</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
@@ -1969,19 +1973,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" t="s">
         <v>134</v>
-      </c>
-      <c r="B12" t="s">
-        <v>135</v>
       </c>
       <c r="C12">
         <v>13269292</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -1989,16 +1993,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C13">
         <v>13866117</v>
       </c>
       <c r="E13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
@@ -2006,19 +2010,19 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" t="s">
         <v>137</v>
-      </c>
-      <c r="B14" t="s">
-        <v>138</v>
       </c>
       <c r="C14">
         <v>4056210</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
@@ -2026,16 +2030,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="s">
         <v>140</v>
-      </c>
-      <c r="B15" t="s">
-        <v>141</v>
       </c>
       <c r="C15">
         <v>8127339</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
@@ -2043,16 +2047,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="s">
         <v>143</v>
-      </c>
-      <c r="B16" t="s">
-        <v>144</v>
       </c>
       <c r="C16">
         <v>8397896</v>
       </c>
       <c r="E16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -2060,19 +2064,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C17">
         <v>4475</v>
       </c>
       <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" t="s">
         <v>149</v>
-      </c>
-      <c r="E17" t="s">
-        <v>150</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -2080,16 +2084,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18">
         <v>32220</v>
       </c>
       <c r="E18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
@@ -2097,19 +2101,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" t="s">
         <v>152</v>
-      </c>
-      <c r="B19" t="s">
-        <v>153</v>
       </c>
       <c r="C19">
         <v>8181484</v>
       </c>
       <c r="D19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" t="s">
         <v>154</v>
-      </c>
-      <c r="E19" t="s">
-        <v>155</v>
       </c>
       <c r="F19" t="s">
         <v>12</v>
@@ -2117,16 +2121,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" t="s">
         <v>158</v>
-      </c>
-      <c r="B20" t="s">
-        <v>159</v>
       </c>
       <c r="C20">
         <v>27365</v>
       </c>
       <c r="E20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>

</xml_diff>